<commit_message>
RDM-2237 Updates after merging master
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V35_RDM-2237.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V35_RDM-2237.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="29005"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/src/ccd/temp/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/space/workspace/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E83E896-0531-2B4C-A59F-F16EFA52C4D6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5640" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="294">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -936,11 +937,17 @@
   <si>
     <t>5,10,15</t>
   </si>
+  <si>
+    <t>Boolean value to say if the current values entered for the event can be saved as draft (Valid only for Create Events)</t>
+  </si>
+  <si>
+    <t>CanSaveDraft</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
@@ -2036,7 +2043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2262,7 +2269,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2624,7 +2631,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2938,7 +2945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -3301,7 +3308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -4042,7 +4049,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
@@ -4240,8 +4247,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4252,7 +4259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:IU10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -6919,10 +6926,10 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -7933,7 +7940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:IU15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -11961,7 +11968,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -12845,7 +12852,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -13213,7 +13220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -14571,7 +14578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
@@ -14916,7 +14923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -15840,7 +15847,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -16220,11 +16227,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16246,7 +16253,10 @@
     <col min="15" max="15" width="29.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="23.6640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="31.1640625" style="1" customWidth="1"/>
-    <col min="18" max="21" width="8.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.83203125" style="1" customWidth="1"/>
     <col min="22" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16278,7 +16288,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="T1" s="120"/>
       <c r="U1" s="4"/>
     </row>
     <row r="2" spans="1:21" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -16335,7 +16345,9 @@
       <c r="S2" s="130" t="s">
         <v>277</v>
       </c>
-      <c r="T2" s="5"/>
+      <c r="T2" s="130" t="s">
+        <v>292</v>
+      </c>
       <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16396,7 +16408,9 @@
       <c r="S3" s="131" t="s">
         <v>278</v>
       </c>
-      <c r="T3" s="8"/>
+      <c r="T3" s="131" t="s">
+        <v>293</v>
+      </c>
       <c r="U3" s="8"/>
     </row>
     <row r="4" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16445,7 +16459,9 @@
       <c r="S4" s="120" t="s">
         <v>279</v>
       </c>
-      <c r="T4" s="4"/>
+      <c r="T4" s="120" t="s">
+        <v>172</v>
+      </c>
       <c r="U4" s="4"/>
     </row>
     <row r="5" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16492,7 +16508,7 @@
       <c r="S5" s="120" t="s">
         <v>280</v>
       </c>
-      <c r="T5" s="4"/>
+      <c r="T5" s="120"/>
       <c r="U5" s="4"/>
     </row>
     <row r="6" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16535,7 +16551,7 @@
       </c>
       <c r="R6" s="129"/>
       <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
+      <c r="T6" s="120"/>
       <c r="U6" s="4"/>
     </row>
     <row r="7" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16578,7 +16594,7 @@
         <v>172</v>
       </c>
       <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
+      <c r="T7" s="120"/>
       <c r="U7" s="4"/>
     </row>
     <row r="8" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16623,7 +16639,7 @@
         <v>172</v>
       </c>
       <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
+      <c r="T8" s="120"/>
       <c r="U8" s="4"/>
     </row>
     <row r="9" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16666,7 +16682,7 @@
         <v>172</v>
       </c>
       <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
+      <c r="T9" s="120"/>
       <c r="U9" s="4"/>
     </row>
     <row r="10" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16689,7 +16705,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
+      <c r="T10" s="120"/>
       <c r="U10" s="4"/>
     </row>
     <row r="11" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16712,7 +16728,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
+      <c r="T11" s="120"/>
       <c r="U11" s="4"/>
     </row>
     <row r="12" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16735,7 +16751,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
+      <c r="T12" s="120"/>
       <c r="U12" s="4"/>
     </row>
     <row r="13" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16758,7 +16774,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
+      <c r="T13" s="120"/>
       <c r="U13" s="4"/>
     </row>
     <row r="14" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16781,7 +16797,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
+      <c r="T14" s="120"/>
       <c r="U14" s="4"/>
     </row>
     <row r="15" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16804,7 +16820,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
+      <c r="T15" s="120"/>
       <c r="U15" s="4"/>
     </row>
     <row r="16" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16827,7 +16843,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
+      <c r="T16" s="120"/>
       <c r="U16" s="4"/>
     </row>
     <row r="17" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16850,7 +16866,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
+      <c r="T17" s="120"/>
       <c r="U17" s="4"/>
     </row>
     <row r="18" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16873,7 +16889,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
+      <c r="T18" s="120"/>
       <c r="U18" s="4"/>
     </row>
     <row r="19" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16896,7 +16912,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
+      <c r="T19" s="120"/>
       <c r="U19" s="4"/>
     </row>
   </sheetData>
@@ -16909,7 +16925,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -17586,7 +17602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>

<commit_message>
RDM-2237 codacy complaints addressed
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V35_RDM-2237.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V35_RDM-2237.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/space/workspace/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E83E896-0531-2B4C-A59F-F16EFA52C4D6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6405E11D-727D-5648-A505-6224575425FF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -16230,7 +16230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="L1" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
@@ -16928,8 +16928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17324,7 +17324,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="137" t="s">
-        <v>289</v>
+        <v>195</v>
       </c>
       <c r="L10" s="137"/>
       <c r="M10" s="137"/>

</xml_diff>